<commit_message>
thực hiện kết nối chatbot ai vào đồ án ... cái ni là tìm hiểu ngoài lệ thui ạ
</commit_message>
<xml_diff>
--- a/public/template/template_phongtro.xlsx
+++ b/public/template/template_phongtro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Desktop\QLPhongTro\DungPhongTro\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{459F6FAF-FDAD-4FCF-90A0-1F4A1B442392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36132273-7F1A-472C-A941-FA00FD0329A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F7C1976E-2BF6-4740-AF92-273135DD33EA}"/>
   </bookViews>
@@ -158,15 +158,6 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -177,6 +168,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -559,56 +559,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F69E88C-8B0E-44F1-B0E5-4611A4DF7212}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="20.77734375" style="4"/>
+    <col min="1" max="16384" width="20.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1"/>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="7"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="4"/>
     </row>
-    <row r="2" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="1" t="s">
+    <row r="2" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="3"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="1" t="s">
+    <row r="3" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="3"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="7"/>
     </row>
-    <row r="4" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="1" t="s">
+    <row r="4" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="3"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="C4:H4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>